<commit_message>
test Users added for password reset
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/UserList_ToRest.xlsx
+++ b/src/test/resources/testdata/UserList_ToRest.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="67">
   <si>
     <t>AG1730</t>
   </si>
@@ -129,13 +129,103 @@
     <t>Password</t>
   </si>
   <si>
-    <t>April@2023!</t>
+    <t>Tbrean</t>
+  </si>
+  <si>
+    <t>Bloomis</t>
+  </si>
+  <si>
+    <t>Lrallo</t>
+  </si>
+  <si>
+    <t>Mnickerson</t>
+  </si>
+  <si>
+    <t>Lrambach</t>
+  </si>
+  <si>
+    <t>Jlockwood</t>
+  </si>
+  <si>
+    <t>Tpeck</t>
+  </si>
+  <si>
+    <t>Ckriss</t>
+  </si>
+  <si>
+    <t>Nclay</t>
+  </si>
+  <si>
+    <t>Jritchie</t>
+  </si>
+  <si>
+    <t>CdeGourville</t>
+  </si>
+  <si>
+    <t>Rvanhorn</t>
+  </si>
+  <si>
+    <t>Jbarnes</t>
+  </si>
+  <si>
+    <t>Sunderwood</t>
+  </si>
+  <si>
+    <t>AG1777</t>
+  </si>
+  <si>
+    <t>Ggahrman</t>
+  </si>
+  <si>
+    <t>Lzimmer</t>
+  </si>
+  <si>
+    <t>Dcrouch</t>
+  </si>
+  <si>
+    <t>Kormsby</t>
+  </si>
+  <si>
+    <t>Gwasson</t>
+  </si>
+  <si>
+    <t>Mhammond</t>
+  </si>
+  <si>
+    <t>Ccastillo</t>
+  </si>
+  <si>
+    <t>Tsimmons</t>
+  </si>
+  <si>
+    <t>Dgaldiano</t>
+  </si>
+  <si>
+    <t>Jhall</t>
+  </si>
+  <si>
+    <t>Tbrydon</t>
+  </si>
+  <si>
+    <t>AG8166</t>
+  </si>
+  <si>
+    <t>AG0376</t>
+  </si>
+  <si>
+    <t>AG8735</t>
+  </si>
+  <si>
+    <t>AG1529A2</t>
+  </si>
+  <si>
+    <t>May@2023!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -510,19 +600,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="2" max="2" width="19.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -530,279 +620,543 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B35" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="B36" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A52" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A59" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A60" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A61" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A62" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A63" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A64" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A65" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A66" s="2"/>
+      <c r="B66" s="5"/>
+    </row>
+    <row r="67" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A67" s="2"/>
+      <c r="B67" s="5"/>
+    </row>
+    <row r="68" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A68" s="2"/>
+      <c r="B68" s="5"/>
+    </row>
+    <row r="69" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A69" s="2"/>
+      <c r="B69" s="5"/>
+    </row>
+    <row r="70" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A70" s="2"/>
+      <c r="B70" s="5"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3:B65" r:id="rId2" display="May@2023!"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>